<commit_message>
Translated Checklist and Report Template to Japanese.
</commit_message>
<xml_diff>
--- a/Checklist_JP.xlsx
+++ b/Checklist_JP.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9934E05C-C095-4F9B-9A0B-359766731E26}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C263EF0-9A83-4F67-AD18-FA3DC30B24D3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="13515" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ワークフロー" sheetId="2" r:id="rId1"/>
@@ -43,83 +43,23 @@
     <phoneticPr fontId="6"/>
   </si>
   <si>
-    <t>Missing workflow annotation</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>The top level activity (usually a flowchart or sequence) of a workflow should have a brief textual description giving an overview of its purpose. This helps developers to quickly understand the workflow's goal, inputs, outputs, preconditions and outcomes.</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
     <t>Checks\MissingWorkflowAnnotation.xaml</t>
     <phoneticPr fontId="6"/>
   </si>
   <si>
-    <t>Missing screenshot</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
     <t>Checks\MissingScreenshot.xaml</t>
     <phoneticPr fontId="6"/>
   </si>
   <si>
-    <t>Other than textual descriptions, screenshots are helpful in explaining what the activity does and with what elements it interacts. The screenshots should be stored in the .screenshots folder of the project.</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Consider adding a reference screenshot.</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Consider adding a brief description of the workflow as an annotation in the top level activity.</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Undocumented delay</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Consider using other mechanisms to wait for application states. When it is absolutely necessary to use Delays, add annotations that explain why they are being used.</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Delays may unnecessarily affect overall robot performance, and therefore their use should be limited to a minimum. For more about synchronization, refer to https://studio.uipath.com/docs/ui-automation#section-ui-synchronization</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
     <t>Checks\UndocumentedDelay.xaml</t>
     <phoneticPr fontId="6"/>
   </si>
   <si>
-    <t>Empty Catch block</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
     <t>Checks\EmptyCatchBlock.xaml</t>
     <phoneticPr fontId="6"/>
   </si>
   <si>
-    <t>Exceptions should be caught with a purpose, not only to prevent error messages. For this reason, it is recommended to insert log messages in the Catch block of a Try Catch activity, in addition to the exception handling itself. For more about error handling, refer to https://studio.uipath.com/docs/project-organization#section-error-handling</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>If no action is taken to handle the exception, include at least a Log Message activity and Rethrow it.</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Variables not following naming convention</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
     <t>Checks\VariableNamingConvention.xaml</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Make sure all the variables follow the project's naming convention.</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Variables in a project should follow a specified naming convention, since it makes it easier to understand the project and maintain it. This check receives a regular expression that dictates the naming convention for variables. For more information about naming conventions, refer to https://studio.uipath.com/docs/workflow-design#section-naming-conventions</t>
     <phoneticPr fontId="6"/>
   </si>
   <si>
@@ -127,19 +67,7 @@
     <phoneticPr fontId="5"/>
   </si>
   <si>
-    <t>Arguments not following naming convention</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Make sure all the arguments follow the project's naming convention.</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
     <t>Checks\ArgumentNamingConvention.xaml</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Arguments in a project should follow a specified naming convention, since it makes it easier to understand the project and maintain it. This check receives a regular expression that dictates the naming convention for arguments. For more information about naming conventions, refer to https://studio.uipath.com/docs/workflow-design#section-naming-conventions</t>
     <phoneticPr fontId="6"/>
   </si>
   <si>
@@ -147,59 +75,15 @@
     <phoneticPr fontId="5"/>
   </si>
   <si>
-    <t>SimulateClick not used</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
     <t>Checks\UseSimulateClick.xaml</t>
     <phoneticPr fontId="6"/>
   </si>
   <si>
-    <t>Since it does not depend on the mouse driver, SimulateClick provides a faster and more robust way to perform clicks, so it should be used whenever possible. For more about input methods, refer to https://studio.uipath.com/docs/ui-automation#section-input-methods</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Use SimulateClick if the target control supports it.</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>SimulateType not used</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
     <t>Checks\UseSimulateType.xaml</t>
     <phoneticPr fontId="6"/>
   </si>
   <si>
-    <t>Since it does not depend on the keyboard driver, SimulateType provides a faster and more robust way to perform type actions, so it should be used whenever possible. For more about input methods, refer to https://studio.uipath.com/docs/ui-automation#section-input-methods</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Use SimulateType if the target control supports it.</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>The idx attribute is used to distinguish elements with the same selector based on their order in the interface hierarchy. This order can change if the elements on the screen change, so the value for the idx attribute should be kept to a low value to avoid the selection of wrong elements. This checks receives a threshold for the value of the idx attribute. For more about selectors, refer to https://studio.uipath.com/docs/ui-automation#section-selectors</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Consider using other attributes in the selector to make it less dependent on the idx attribute. </t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Use of large idx value in selector</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
     <t>Checks\LargeIdxInSelector.xaml</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>The project.json file contains important information about the project and it is used by UiPath Studio when loading the project. For more information about this file, refer to https://studio.uipath.com/docs/about-the-projectjson-file</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Create or import a project.json file for the project.</t>
     <phoneticPr fontId="6"/>
   </si>
   <si>
@@ -218,39 +102,881 @@
     <phoneticPr fontId="5"/>
   </si>
   <si>
-    <t>No project configuration file (project.json) found</t>
+    <t>Checks\UnnecessarySequenceOrFlowchart.xaml</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Checks\UnreachableActivities.xaml</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>最上位階層のアクティビティ（基本的にFlowchartやSequence）には、ワークフローの目的・概要を簡潔に注釈することを推奨します。これにより、開発者はワークフローの目的・インプット・アウトプット・前提条件を素早く把握することができます。</t>
+    <rPh sb="0" eb="3">
+      <t>サイジョウイ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>カイソウ</t>
+    </rPh>
+    <rPh sb="14" eb="17">
+      <t>キホンテキ</t>
+    </rPh>
+    <rPh sb="47" eb="49">
+      <t>モクテキ</t>
+    </rPh>
+    <rPh sb="50" eb="52">
+      <t>ガイヨウ</t>
+    </rPh>
+    <rPh sb="53" eb="55">
+      <t>カンケツ</t>
+    </rPh>
+    <rPh sb="56" eb="58">
+      <t>チュウシャク</t>
+    </rPh>
+    <rPh sb="63" eb="65">
+      <t>スイショウ</t>
+    </rPh>
+    <rPh sb="75" eb="78">
+      <t>カイハツシャ</t>
+    </rPh>
+    <rPh sb="86" eb="88">
+      <t>モクテキ</t>
+    </rPh>
+    <rPh sb="102" eb="104">
+      <t>ゼンテイ</t>
+    </rPh>
+    <rPh sb="104" eb="106">
+      <t>ジョウケン</t>
+    </rPh>
+    <rPh sb="107" eb="109">
+      <t>スバヤ</t>
+    </rPh>
+    <rPh sb="110" eb="112">
+      <t>ハアク</t>
+    </rPh>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>最上位階層のアクティビティには、ワークフローの概要を注釈することを推奨します。</t>
+    <rPh sb="0" eb="3">
+      <t>サイジョウイ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>カイソウ</t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t>ガイヨウ</t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t>チュウシャク</t>
+    </rPh>
+    <rPh sb="33" eb="35">
+      <t>スイショウ</t>
+    </rPh>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>注釈の欠落</t>
+    <rPh sb="0" eb="2">
+      <t>チュウシャク</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ケツラク</t>
+    </rPh>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>スクリーンショットの欠落</t>
+    <rPh sb="10" eb="12">
+      <t>ケツラク</t>
+    </rPh>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>スクリーンショットは、アクティビティがどの要素に対してどういった処理を実行するか確認するのに有効です。各スクリーンショットは、プロジェクト内の「.screenshots」フォルダに、保存されている必要があります。</t>
+    <rPh sb="21" eb="23">
+      <t>ヨウソ</t>
+    </rPh>
+    <rPh sb="24" eb="25">
+      <t>タイ</t>
+    </rPh>
+    <rPh sb="32" eb="34">
+      <t>ショリ</t>
+    </rPh>
+    <rPh sb="35" eb="37">
+      <t>ジッコウ</t>
+    </rPh>
+    <rPh sb="40" eb="42">
+      <t>カクニン</t>
+    </rPh>
+    <rPh sb="46" eb="48">
+      <t>ユウコウ</t>
+    </rPh>
+    <rPh sb="51" eb="52">
+      <t>カク</t>
+    </rPh>
+    <rPh sb="69" eb="70">
+      <t>ナイ</t>
+    </rPh>
+    <rPh sb="91" eb="93">
+      <t>ホゾン</t>
+    </rPh>
+    <rPh sb="98" eb="100">
+      <t>ヒツヨウ</t>
+    </rPh>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>有効なスクリーンショットを参照してください。</t>
+    <rPh sb="0" eb="2">
+      <t>ユウコウ</t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t>サンショウ</t>
+    </rPh>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>注釈の無い待機（Delay）</t>
+    <rPh sb="0" eb="2">
+      <t>チュウシャク</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>ナ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>タイキ</t>
+    </rPh>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>待機（Delay）は、必要以上にロボットのパフォーマンスを低下させることがあるので、その使用は最小限にすることを推奨しています。UI同期の方法は、待機（Delay）以外の方法を含めて、こちらのページで紹介されています。https://studio.uipath.com/lang-ja/docs/ui-automation#section-ui-synchronization</t>
+    <rPh sb="0" eb="2">
+      <t>タイキ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>ヒツヨウ</t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t>イジョウ</t>
+    </rPh>
+    <rPh sb="29" eb="31">
+      <t>テイカ</t>
+    </rPh>
+    <rPh sb="44" eb="46">
+      <t>シヨウ</t>
+    </rPh>
+    <rPh sb="47" eb="50">
+      <t>サイショウゲン</t>
+    </rPh>
+    <rPh sb="56" eb="58">
+      <t>スイショウ</t>
+    </rPh>
+    <rPh sb="66" eb="68">
+      <t>ドウキ</t>
+    </rPh>
+    <rPh sb="69" eb="71">
+      <t>ホウホウ</t>
+    </rPh>
+    <rPh sb="73" eb="75">
+      <t>タイキ</t>
+    </rPh>
+    <rPh sb="82" eb="84">
+      <t>イガイ</t>
+    </rPh>
+    <rPh sb="85" eb="87">
+      <t>ホウホウ</t>
+    </rPh>
+    <rPh sb="88" eb="89">
+      <t>フク</t>
+    </rPh>
+    <rPh sb="100" eb="102">
+      <t>ショウカイ</t>
+    </rPh>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>アプリケーションの状態変化を待つ方法として、待機（Delay）以外を検討してください。待機（Delay）が絶対に必要な状況の場合は、その理由を注釈に記載してください。</t>
+    <rPh sb="9" eb="11">
+      <t>ジョウタイ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>ヘンカ</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>マ</t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t>ホウホウ</t>
+    </rPh>
+    <rPh sb="43" eb="45">
+      <t>タイキ</t>
+    </rPh>
+    <rPh sb="53" eb="55">
+      <t>ゼッタイ</t>
+    </rPh>
+    <rPh sb="56" eb="58">
+      <t>ヒツヨウ</t>
+    </rPh>
+    <rPh sb="59" eb="61">
+      <t>ジョウキョウ</t>
+    </rPh>
+    <rPh sb="62" eb="64">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="68" eb="70">
+      <t>リユウ</t>
+    </rPh>
+    <rPh sb="71" eb="73">
+      <t>チュウシャク</t>
+    </rPh>
+    <rPh sb="74" eb="76">
+      <t>キサイ</t>
+    </rPh>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>空のキャッチ（Catch）ブロック</t>
+    <rPh sb="0" eb="1">
+      <t>カラ</t>
+    </rPh>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>例外のキャッチは、ただエラーメッセージを回避するためでなく、目的を持って行われるべきです。そのため、トライキャッチ（Try Catch）のキャッチブロックには、ログメッセージの出力を推奨しています。エラー処理に関する情報はこちらのページで紹介されています。 https://studio.uipath.com/lang-ja/docs/project-organization#section-error-handling</t>
+    <rPh sb="0" eb="2">
+      <t>レイガイ</t>
+    </rPh>
+    <rPh sb="20" eb="22">
+      <t>カイヒ</t>
+    </rPh>
+    <rPh sb="30" eb="32">
+      <t>モクテキ</t>
+    </rPh>
+    <rPh sb="33" eb="34">
+      <t>モ</t>
+    </rPh>
+    <rPh sb="36" eb="37">
+      <t>オコナ</t>
+    </rPh>
+    <rPh sb="88" eb="90">
+      <t>シュツリョク</t>
+    </rPh>
+    <rPh sb="91" eb="93">
+      <t>スイショウ</t>
+    </rPh>
+    <rPh sb="102" eb="104">
+      <t>ショリ</t>
+    </rPh>
+    <rPh sb="105" eb="106">
+      <t>カン</t>
+    </rPh>
+    <rPh sb="108" eb="110">
+      <t>ジョウホウ</t>
+    </rPh>
+    <rPh sb="119" eb="121">
+      <t>ショウカイ</t>
+    </rPh>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>例外をキャッチした際に対応することがない場合でも、少なくともログメッセージを出力することを推奨します。</t>
+    <rPh sb="0" eb="2">
+      <t>レイガイ</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>サイ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>タイオウ</t>
+    </rPh>
+    <rPh sb="20" eb="22">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="25" eb="26">
+      <t>スク</t>
+    </rPh>
+    <rPh sb="38" eb="40">
+      <t>シュツリョク</t>
+    </rPh>
+    <rPh sb="45" eb="47">
+      <t>スイショウ</t>
+    </rPh>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>命名規則違反（変数）</t>
+    <rPh sb="0" eb="2">
+      <t>メイメイ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>キソク</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>イハン</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>ヘンスウ</t>
+    </rPh>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>命名規則違反（引数）</t>
+    <rPh sb="0" eb="2">
+      <t>メイメイ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>キソク</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>イハン</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>ヒキスウ</t>
+    </rPh>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>変数の命名は、ワークフローの保守性を維持するため、指定された命名規則を守る必要があります。こちらのチェックは、正規表現を引数として受け取り、それを守っているかどうかを確認する機能となります。命名規則に関してはこちらのページで紹介されています。 https://studio.uipath.com/lang-ja/docs/workflow-design#section-naming-conventions</t>
+    <rPh sb="0" eb="2">
+      <t>ヘンスウ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>メイメイ</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>ホシュ</t>
+    </rPh>
+    <rPh sb="16" eb="17">
+      <t>セイ</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>イジ</t>
+    </rPh>
+    <rPh sb="25" eb="27">
+      <t>シテイ</t>
+    </rPh>
+    <rPh sb="30" eb="32">
+      <t>メイメイ</t>
+    </rPh>
+    <rPh sb="32" eb="34">
+      <t>キソク</t>
+    </rPh>
+    <rPh sb="35" eb="36">
+      <t>マモ</t>
+    </rPh>
+    <rPh sb="37" eb="39">
+      <t>ヒツヨウ</t>
+    </rPh>
+    <rPh sb="55" eb="57">
+      <t>セイキ</t>
+    </rPh>
+    <rPh sb="57" eb="59">
+      <t>ヒョウゲン</t>
+    </rPh>
+    <rPh sb="60" eb="62">
+      <t>ヒキスウ</t>
+    </rPh>
+    <rPh sb="65" eb="66">
+      <t>ウ</t>
+    </rPh>
+    <rPh sb="67" eb="68">
+      <t>ト</t>
+    </rPh>
+    <rPh sb="73" eb="74">
+      <t>マモ</t>
+    </rPh>
+    <rPh sb="83" eb="85">
+      <t>カクニン</t>
+    </rPh>
+    <rPh sb="87" eb="89">
+      <t>キノウ</t>
+    </rPh>
+    <rPh sb="95" eb="97">
+      <t>メイメイ</t>
+    </rPh>
+    <rPh sb="97" eb="99">
+      <t>キソク</t>
+    </rPh>
+    <rPh sb="100" eb="101">
+      <t>カン</t>
+    </rPh>
+    <rPh sb="112" eb="114">
+      <t>ショウカイ</t>
+    </rPh>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>引数の命名は、ワークフローの保守性を維持するため、指定された命名規則を守る必要があります。こちらのチェックは、正規表現を引数として受け取り、それを守っているかどうかを確認する機能となります。命名規則に関してはこちらのページで紹介されています。 https://studio.uipath.com/lang-ja/docs/workflow-design#section-naming-conventions</t>
+    <rPh sb="0" eb="2">
+      <t>ヒキスウ</t>
+    </rPh>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>変数名は命名規則に従って命名してください。</t>
+    <rPh sb="0" eb="3">
+      <t>ヘンスウメイ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>メイメイ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>キソク</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>シタガ</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>メイメイ</t>
+    </rPh>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>引数名は命名規則に従って命名してください。</t>
+    <rPh sb="0" eb="2">
+      <t>ヒキスウ</t>
+    </rPh>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>クリックをシミュレート（SimulateClick）の不使用</t>
+    <rPh sb="27" eb="30">
+      <t>フシヨウ</t>
+    </rPh>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>入力をシミュレート（SimulateType）の不使用</t>
+    <rPh sb="0" eb="2">
+      <t>ニュウリョク</t>
+    </rPh>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>クリックをシミュレート（SimulateClick）は、マウスドライバーを使用しないため、より高速で安定したクリックを実行することができます。そのため、このオプションを使用して正常に動作する場合は、常に使用することを推奨します。 クリックをシミュレート（SimulateClick）については、こちらのページで紹介されています。https://studio.uipath.com/lang-ja/docs/ui-automation#section-input-methods</t>
+    <rPh sb="37" eb="39">
+      <t>シヨウ</t>
+    </rPh>
+    <rPh sb="47" eb="49">
+      <t>コウソク</t>
+    </rPh>
+    <rPh sb="50" eb="52">
+      <t>アンテイ</t>
+    </rPh>
+    <rPh sb="59" eb="61">
+      <t>ジッコウ</t>
+    </rPh>
+    <rPh sb="84" eb="86">
+      <t>シヨウ</t>
+    </rPh>
+    <rPh sb="88" eb="90">
+      <t>セイジョウ</t>
+    </rPh>
+    <rPh sb="91" eb="93">
+      <t>ドウサ</t>
+    </rPh>
+    <rPh sb="95" eb="97">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="99" eb="100">
+      <t>ツネ</t>
+    </rPh>
+    <rPh sb="101" eb="103">
+      <t>シヨウ</t>
+    </rPh>
+    <rPh sb="108" eb="110">
+      <t>スイショウ</t>
+    </rPh>
+    <rPh sb="155" eb="157">
+      <t>ショウカイ</t>
+    </rPh>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>入力をシミュレート（SimulateType）は、キーボードドライバーを使用しないため、より高速で安定した入力を実行することができます。そのため、このオプションを使用して正常に動作する場合は、常に使用することを推奨します。 入力をシミュレート（SimulateType）については、こちらのページで紹介されています。 https://studio.uipath.com/lang-ja/docs/ui-automation#section-input-methods</t>
+    <rPh sb="0" eb="2">
+      <t>ニュウリョク</t>
+    </rPh>
+    <rPh sb="53" eb="55">
+      <t>ニュウリョク</t>
+    </rPh>
+    <rPh sb="112" eb="114">
+      <t>ニュウリョク</t>
+    </rPh>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>正常に動作しない場合を除き、クリックをシミュレート（SimulateClick）を使用することを推奨します。</t>
+    <rPh sb="0" eb="2">
+      <t>セイジョウ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ドウサ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>ノゾ</t>
+    </rPh>
+    <rPh sb="41" eb="43">
+      <t>シヨウ</t>
+    </rPh>
+    <rPh sb="48" eb="50">
+      <t>スイショウ</t>
+    </rPh>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>正常に動作しない場合を除き、入力をシミュレート（SimulateType）を使用することを推奨します。</t>
+    <rPh sb="14" eb="16">
+      <t>ニュウリョク</t>
+    </rPh>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>idx属性値が大きいので、セレクターにidx属性以外の属性を追加することを検討してください。</t>
+    <rPh sb="3" eb="5">
+      <t>ゾクセイ</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>チ</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>オオ</t>
+    </rPh>
+    <rPh sb="22" eb="24">
+      <t>ゾクセイ</t>
+    </rPh>
+    <rPh sb="27" eb="29">
+      <t>ゾクセイ</t>
+    </rPh>
+    <rPh sb="30" eb="32">
+      <t>ツイカ</t>
+    </rPh>
+    <rPh sb="37" eb="39">
+      <t>ケントウ</t>
+    </rPh>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>セレクターのidx属性は、同じセレクターで取得できる要素を、要素の順序に基づいて判別するために使われます。この順序は、画面の要素が変わると、それに伴って変わってしまうことがあります。誤った要素を選択することを避けるため、idx属性の値はできるだけ小さい値となるようにセレクターを構築することを推奨します。こちらのチェックは、引数としてidx属性の閾値を受け取り、その値より大きいか確認しています。セレクターについてはこちらのページで紹介されています。 https://studio.uipath.com/lang-ja/docs/ui-automation#section-selectors</t>
+    <rPh sb="9" eb="11">
+      <t>ゾクセイ</t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t>オナ</t>
+    </rPh>
+    <rPh sb="21" eb="23">
+      <t>シュトク</t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t>ヨウソ</t>
+    </rPh>
+    <rPh sb="30" eb="32">
+      <t>ヨウソ</t>
+    </rPh>
+    <rPh sb="33" eb="35">
+      <t>ジュンジョ</t>
+    </rPh>
+    <rPh sb="36" eb="37">
+      <t>モト</t>
+    </rPh>
+    <rPh sb="40" eb="42">
+      <t>ハンベツ</t>
+    </rPh>
+    <rPh sb="47" eb="48">
+      <t>ツカ</t>
+    </rPh>
+    <rPh sb="55" eb="57">
+      <t>ジュンジョ</t>
+    </rPh>
+    <rPh sb="59" eb="61">
+      <t>ガメン</t>
+    </rPh>
+    <rPh sb="62" eb="64">
+      <t>ヨウソ</t>
+    </rPh>
+    <rPh sb="65" eb="66">
+      <t>カ</t>
+    </rPh>
+    <rPh sb="73" eb="74">
+      <t>トモナ</t>
+    </rPh>
+    <rPh sb="76" eb="77">
+      <t>カ</t>
+    </rPh>
+    <rPh sb="91" eb="92">
+      <t>アヤマ</t>
+    </rPh>
+    <rPh sb="94" eb="96">
+      <t>ヨウソ</t>
+    </rPh>
+    <rPh sb="97" eb="99">
+      <t>センタク</t>
+    </rPh>
+    <rPh sb="104" eb="105">
+      <t>サ</t>
+    </rPh>
+    <rPh sb="113" eb="115">
+      <t>ゾクセイ</t>
+    </rPh>
+    <rPh sb="116" eb="117">
+      <t>アタイ</t>
+    </rPh>
+    <rPh sb="123" eb="124">
+      <t>チイ</t>
+    </rPh>
+    <rPh sb="126" eb="127">
+      <t>アタイ</t>
+    </rPh>
+    <rPh sb="139" eb="141">
+      <t>コウチク</t>
+    </rPh>
+    <rPh sb="146" eb="148">
+      <t>スイショウ</t>
+    </rPh>
+    <rPh sb="162" eb="164">
+      <t>ヒキスウ</t>
+    </rPh>
+    <rPh sb="170" eb="172">
+      <t>ゾクセイ</t>
+    </rPh>
+    <rPh sb="173" eb="175">
+      <t>イキチ</t>
+    </rPh>
+    <rPh sb="176" eb="177">
+      <t>ウ</t>
+    </rPh>
+    <rPh sb="178" eb="179">
+      <t>ト</t>
+    </rPh>
+    <rPh sb="183" eb="184">
+      <t>アタイ</t>
+    </rPh>
+    <rPh sb="186" eb="187">
+      <t>オオ</t>
+    </rPh>
+    <rPh sb="190" eb="192">
+      <t>カクニン</t>
+    </rPh>
+    <rPh sb="216" eb="218">
+      <t>ショウカイ</t>
+    </rPh>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>セレクターのidx属性値が過大</t>
+    <rPh sb="9" eb="11">
+      <t>ゾクセイ</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>チ</t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t>カダイ</t>
+    </rPh>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>不必要なシーケンス（Sequence）やフローチャート（Flowchart）</t>
+    <rPh sb="0" eb="3">
+      <t>フヒツヨウ</t>
+    </rPh>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>実行されないアクティビティ</t>
+    <rPh sb="0" eb="2">
+      <t>ジッコウ</t>
+    </rPh>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>ワークフロー上において、シーケンスは特定の目的を果たすために使用されます。そのため、空のシーケンスは、ワークフローの可読性を低めるだけなので、使用されるべきではありません。また、内部にアクティビティを１つしか含まないシーケンスやフローチャートは、基本的に削除してもワークフローの動作に影響を及ぼしません。 シーケンスの削除には、 コンテキストメニューのシーケンスを削除（Remove Sequence）オプションを使用することができます。 (https://studio.uipath.com/lang-ja/docs/the-user-interface#section-the-context-menu).</t>
+    <rPh sb="6" eb="7">
+      <t>ジョウ</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>トクテイ</t>
+    </rPh>
+    <rPh sb="21" eb="23">
+      <t>モクテキ</t>
+    </rPh>
+    <rPh sb="24" eb="25">
+      <t>ハ</t>
+    </rPh>
+    <rPh sb="30" eb="32">
+      <t>シヨウ</t>
+    </rPh>
+    <rPh sb="42" eb="43">
+      <t>カラ</t>
+    </rPh>
+    <rPh sb="58" eb="61">
+      <t>カドクセイ</t>
+    </rPh>
+    <rPh sb="62" eb="63">
+      <t>ヒク</t>
+    </rPh>
+    <rPh sb="71" eb="73">
+      <t>シヨウ</t>
+    </rPh>
+    <rPh sb="89" eb="91">
+      <t>ナイブ</t>
+    </rPh>
+    <rPh sb="104" eb="105">
+      <t>フク</t>
+    </rPh>
+    <rPh sb="123" eb="126">
+      <t>キホンテキ</t>
+    </rPh>
+    <rPh sb="127" eb="129">
+      <t>サクジョ</t>
+    </rPh>
+    <rPh sb="139" eb="141">
+      <t>ドウサ</t>
+    </rPh>
+    <rPh sb="142" eb="144">
+      <t>エイキョウ</t>
+    </rPh>
+    <rPh sb="145" eb="146">
+      <t>オヨ</t>
+    </rPh>
+    <rPh sb="159" eb="161">
+      <t>サクジョ</t>
+    </rPh>
+    <rPh sb="182" eb="184">
+      <t>サクジョ</t>
+    </rPh>
+    <rPh sb="207" eb="209">
+      <t>シヨウ</t>
+    </rPh>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>実行されないアクティビティの削除を検討してください。</t>
+    <rPh sb="0" eb="2">
+      <t>ジッコウ</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>サクジョ</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>ケントウ</t>
+    </rPh>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>空の、もしくは、内部にアクティビティを1つしか含まないシーケンス・フローチャートの削除を検討してください。</t>
+    <rPh sb="0" eb="1">
+      <t>カラ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>ナイブ</t>
+    </rPh>
+    <rPh sb="23" eb="24">
+      <t>フク</t>
+    </rPh>
+    <rPh sb="41" eb="43">
+      <t>サクジョ</t>
+    </rPh>
+    <rPh sb="44" eb="46">
+      <t>ケントウ</t>
+    </rPh>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>ワークフロー上には、実行時に必要なアクティビティのみ配置されるべきです。コメントアウトされたアクティビティや、フローチャート上でどのノードにも接続されていないアクティビティは削除することを推奨します。コメントアウトしたアクティビティを保持することが必要な場合は、その理由を注釈してください。</t>
+    <rPh sb="6" eb="7">
+      <t>ジョウ</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>ジッコウ</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>ジ</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>ヒツヨウ</t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t>ハイチ</t>
+    </rPh>
+    <rPh sb="62" eb="63">
+      <t>ジョウ</t>
+    </rPh>
+    <rPh sb="71" eb="73">
+      <t>セツゾク</t>
+    </rPh>
+    <rPh sb="87" eb="89">
+      <t>サクジョ</t>
+    </rPh>
+    <rPh sb="94" eb="96">
+      <t>スイショウ</t>
+    </rPh>
+    <rPh sb="117" eb="119">
+      <t>ホジ</t>
+    </rPh>
+    <rPh sb="124" eb="126">
+      <t>ヒツヨウ</t>
+    </rPh>
+    <rPh sb="127" eb="129">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="133" eb="135">
+      <t>リユウ</t>
+    </rPh>
+    <rPh sb="136" eb="138">
+      <t>チュウシャク</t>
+    </rPh>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>プロジェクト設定ファイル (project.json) の欠落</t>
+    <rPh sb="6" eb="8">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="29" eb="31">
+      <t>ケツラク</t>
+    </rPh>
     <phoneticPr fontId="5"/>
   </si>
   <si>
-    <t>Workflows should only contain sequences that are being used for a specific purpose. Empty sequences should not be used, since they only make the workflow cluttered. In addition, sequences or workflows that contain only one internal activity (even if it is another sequence) can usually be removed without any impact on the functionality of the project. For removing sequences, use the Remove Sequence option of the Context Menu in UiPath Studio (https://studio.uipath.com/docs/the-user-interface#section-the-context-menu).</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Unnecessary sequence or flowchart</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Checks\UnnecessarySequenceOrFlowchart.xaml</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Remove sequences or flowcharts that are empty or contain only one activity.</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Workflows should only have the necessary activities for its execution, and activities that are commented out or that are not connected to any node in a flowchart should be removed. If there is need to keep commented activities, add annotations to describe the reason.</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Consider removing unreachable activities.</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Unreachable activities</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Checks\UnreachableActivities.xaml</t>
+    <t>project.jsonファイルには、プロジェクトに関する重要な情報が含まれており、UiPathStudioでプロジェクトを読み込む際に使用されています。 project.jsonファイルについてはこちらのページで紹介されています。 https://studio.uipath.com/lang-ja/docs/about-the-projectjson-file</t>
+    <rPh sb="26" eb="27">
+      <t>カン</t>
+    </rPh>
+    <rPh sb="29" eb="31">
+      <t>ジュウヨウ</t>
+    </rPh>
+    <rPh sb="32" eb="34">
+      <t>ジョウホウ</t>
+    </rPh>
+    <rPh sb="35" eb="36">
+      <t>フク</t>
+    </rPh>
+    <rPh sb="62" eb="63">
+      <t>ヨ</t>
+    </rPh>
+    <rPh sb="64" eb="65">
+      <t>コ</t>
+    </rPh>
+    <rPh sb="66" eb="67">
+      <t>サイ</t>
+    </rPh>
+    <rPh sb="68" eb="70">
+      <t>シヨウ</t>
+    </rPh>
+    <rPh sb="107" eb="109">
+      <t>ショウカイ</t>
+    </rPh>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>project.jsonファイルを作成もしくはインポートしてください。</t>
+    <rPh sb="17" eb="19">
+      <t>サクセイ</t>
+    </rPh>
     <phoneticPr fontId="6"/>
   </si>
 </sst>
@@ -441,7 +1167,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="標準" xfId="0" builtinId="0"/>
     <cellStyle name="標準 2" xfId="1" xr:uid="{FACCEB44-97B3-401B-BD48-08626DAD862C}"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -514,13 +1240,13 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>209550</xdr:colOff>
           <xdr:row>1</xdr:row>
-          <xdr:rowOff>485775</xdr:rowOff>
+          <xdr:rowOff>488950</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
           <xdr:colOff>419100</xdr:colOff>
           <xdr:row>1</xdr:row>
-          <xdr:rowOff>733425</xdr:rowOff>
+          <xdr:rowOff>736600</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -581,13 +1307,13 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>190500</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>390525</xdr:rowOff>
+          <xdr:rowOff>393700</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
           <xdr:colOff>400050</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>638175</xdr:rowOff>
+          <xdr:rowOff>641350</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -646,15 +1372,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>219075</xdr:colOff>
+          <xdr:colOff>222250</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>504825</xdr:rowOff>
+          <xdr:rowOff>508000</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
           <xdr:colOff>419100</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>752475</xdr:rowOff>
+          <xdr:rowOff>755650</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -713,7 +1439,7 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>257175</xdr:colOff>
+          <xdr:colOff>260350</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>685800</xdr:rowOff>
         </xdr:from>
@@ -721,7 +1447,7 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>457200</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>923925</xdr:rowOff>
+          <xdr:rowOff>927100</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -780,13 +1506,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>219075</xdr:colOff>
+          <xdr:colOff>222250</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>752475</xdr:rowOff>
+          <xdr:rowOff>755650</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>428625</xdr:colOff>
+          <xdr:colOff>431800</xdr:colOff>
           <xdr:row>5</xdr:row>
           <xdr:rowOff>990600</xdr:rowOff>
         </xdr:to>
@@ -847,13 +1573,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>257175</xdr:colOff>
+          <xdr:colOff>260350</xdr:colOff>
           <xdr:row>6</xdr:row>
-          <xdr:rowOff>809625</xdr:rowOff>
+          <xdr:rowOff>812800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>466725</xdr:colOff>
+          <xdr:colOff>469900</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>1047750</xdr:rowOff>
         </xdr:to>
@@ -920,9 +1646,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>447675</xdr:colOff>
+          <xdr:colOff>450850</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>847725</xdr:rowOff>
+          <xdr:rowOff>850900</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -987,9 +1713,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>447675</xdr:colOff>
+          <xdr:colOff>450850</xdr:colOff>
           <xdr:row>8</xdr:row>
-          <xdr:rowOff>809625</xdr:rowOff>
+          <xdr:rowOff>812800</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1048,7 +1774,7 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>257175</xdr:colOff>
+          <xdr:colOff>260350</xdr:colOff>
           <xdr:row>9</xdr:row>
           <xdr:rowOff>895350</xdr:rowOff>
         </xdr:from>
@@ -1056,7 +1782,7 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>457200</xdr:colOff>
           <xdr:row>9</xdr:row>
-          <xdr:rowOff>1133475</xdr:rowOff>
+          <xdr:rowOff>1136650</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1115,7 +1841,7 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>203200</xdr:colOff>
           <xdr:row>10</xdr:row>
           <xdr:rowOff>1085850</xdr:rowOff>
         </xdr:from>
@@ -1123,7 +1849,7 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>400050</xdr:colOff>
           <xdr:row>10</xdr:row>
-          <xdr:rowOff>1323975</xdr:rowOff>
+          <xdr:rowOff>1327150</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1182,9 +1908,9 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>238125</xdr:colOff>
+          <xdr:colOff>241300</xdr:colOff>
           <xdr:row>11</xdr:row>
-          <xdr:rowOff>276225</xdr:rowOff>
+          <xdr:rowOff>279400</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
@@ -1256,11 +1982,11 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>228600</xdr:colOff>
           <xdr:row>1</xdr:row>
-          <xdr:rowOff>447675</xdr:rowOff>
+          <xdr:rowOff>450850</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>428625</xdr:colOff>
+          <xdr:colOff>431800</xdr:colOff>
           <xdr:row>1</xdr:row>
           <xdr:rowOff>685800</xdr:rowOff>
         </xdr:to>
@@ -1584,24 +2310,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBC94E0F-66AD-4ECB-A9C2-26293DFAAC50}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" width="8.625" style="1"/>
-    <col min="2" max="2" width="15.625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="28.375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="49.875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="39.625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.625" style="1"/>
+    <col min="1" max="1" width="8.58203125" style="1"/>
+    <col min="2" max="2" width="15.58203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="28.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="49.83203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="39.58203125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.58203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
-        <v>46</v>
+        <v>17</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>4</v>
@@ -1619,208 +2343,208 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="5" customFormat="1" ht="93.75">
+    <row r="2" spans="1:6" s="5" customFormat="1" ht="90">
       <c r="A2" s="10" t="b">
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>5</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>7</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="4" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="5" customFormat="1" ht="75">
+    <row r="3" spans="1:6" s="5" customFormat="1" ht="72">
       <c r="A3" s="10" t="b">
         <v>1</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="4" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="5" customFormat="1" ht="93.75">
+    <row r="4" spans="1:6" s="5" customFormat="1" ht="108">
       <c r="A4" s="10" t="b">
         <v>1</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="4" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="5" customFormat="1" ht="131.25">
+    <row r="5" spans="1:6" s="5" customFormat="1" ht="126">
       <c r="A5" s="11" t="b">
         <v>1</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="4" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="5" customFormat="1" ht="150">
+    <row r="6" spans="1:6" s="5" customFormat="1" ht="126">
       <c r="A6" s="11" t="b">
         <v>1</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="5" customFormat="1" ht="150">
+    <row r="7" spans="1:6" s="5" customFormat="1" ht="126">
       <c r="A7" s="10" t="b">
         <v>1</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="5" customFormat="1" ht="112.5">
+    <row r="8" spans="1:6" s="5" customFormat="1" ht="144">
       <c r="A8" s="10" t="b">
         <v>1</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="4" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="5" customFormat="1" ht="112.5">
+    <row r="9" spans="1:6" s="5" customFormat="1" ht="144">
       <c r="A9" s="10" t="b">
         <v>1</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="4" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="5" customFormat="1" ht="168.75">
+    <row r="10" spans="1:6" s="5" customFormat="1" ht="180">
       <c r="A10" s="10" t="b">
         <v>1</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="D10" s="6">
         <v>2</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="187.5">
+    <row r="11" spans="1:6" ht="180">
       <c r="A11" s="15" t="b">
         <v>1</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="93.75">
+    <row r="12" spans="1:6" ht="108">
       <c r="A12" s="15" t="b">
         <v>1</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>57</v>
+        <v>21</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="4" t="s">
         <v>54</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1841,13 +2565,13 @@
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>209550</xdr:colOff>
                     <xdr:row>1</xdr:row>
-                    <xdr:rowOff>485775</xdr:rowOff>
+                    <xdr:rowOff>488950</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>419100</xdr:colOff>
                     <xdr:row>1</xdr:row>
-                    <xdr:rowOff>733425</xdr:rowOff>
+                    <xdr:rowOff>736600</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -1863,13 +2587,13 @@
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>190500</xdr:colOff>
                     <xdr:row>2</xdr:row>
-                    <xdr:rowOff>390525</xdr:rowOff>
+                    <xdr:rowOff>393700</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>400050</xdr:colOff>
                     <xdr:row>2</xdr:row>
-                    <xdr:rowOff>638175</xdr:rowOff>
+                    <xdr:rowOff>641350</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -1883,15 +2607,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>0</xdr:col>
-                    <xdr:colOff>219075</xdr:colOff>
+                    <xdr:colOff>222250</xdr:colOff>
                     <xdr:row>3</xdr:row>
-                    <xdr:rowOff>504825</xdr:rowOff>
+                    <xdr:rowOff>508000</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>419100</xdr:colOff>
                     <xdr:row>3</xdr:row>
-                    <xdr:rowOff>752475</xdr:rowOff>
+                    <xdr:rowOff>755650</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -1905,7 +2629,7 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>0</xdr:col>
-                    <xdr:colOff>257175</xdr:colOff>
+                    <xdr:colOff>260350</xdr:colOff>
                     <xdr:row>4</xdr:row>
                     <xdr:rowOff>685800</xdr:rowOff>
                   </from>
@@ -1913,7 +2637,7 @@
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>457200</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>923925</xdr:rowOff>
+                    <xdr:rowOff>927100</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -1927,13 +2651,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>0</xdr:col>
-                    <xdr:colOff>219075</xdr:colOff>
+                    <xdr:colOff>222250</xdr:colOff>
                     <xdr:row>5</xdr:row>
-                    <xdr:rowOff>752475</xdr:rowOff>
+                    <xdr:rowOff>755650</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>0</xdr:col>
-                    <xdr:colOff>428625</xdr:colOff>
+                    <xdr:colOff>431800</xdr:colOff>
                     <xdr:row>5</xdr:row>
                     <xdr:rowOff>990600</xdr:rowOff>
                   </to>
@@ -1949,13 +2673,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>0</xdr:col>
-                    <xdr:colOff>257175</xdr:colOff>
+                    <xdr:colOff>260350</xdr:colOff>
                     <xdr:row>6</xdr:row>
-                    <xdr:rowOff>809625</xdr:rowOff>
+                    <xdr:rowOff>812800</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>0</xdr:col>
-                    <xdr:colOff>466725</xdr:colOff>
+                    <xdr:colOff>469900</xdr:colOff>
                     <xdr:row>6</xdr:row>
                     <xdr:rowOff>1047750</xdr:rowOff>
                   </to>
@@ -1977,9 +2701,9 @@
                   </from>
                   <to>
                     <xdr:col>0</xdr:col>
-                    <xdr:colOff>447675</xdr:colOff>
+                    <xdr:colOff>450850</xdr:colOff>
                     <xdr:row>7</xdr:row>
-                    <xdr:rowOff>847725</xdr:rowOff>
+                    <xdr:rowOff>850900</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -1999,9 +2723,9 @@
                   </from>
                   <to>
                     <xdr:col>0</xdr:col>
-                    <xdr:colOff>447675</xdr:colOff>
+                    <xdr:colOff>450850</xdr:colOff>
                     <xdr:row>8</xdr:row>
-                    <xdr:rowOff>809625</xdr:rowOff>
+                    <xdr:rowOff>812800</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -2015,7 +2739,7 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>0</xdr:col>
-                    <xdr:colOff>257175</xdr:colOff>
+                    <xdr:colOff>260350</xdr:colOff>
                     <xdr:row>9</xdr:row>
                     <xdr:rowOff>895350</xdr:rowOff>
                   </from>
@@ -2023,7 +2747,7 @@
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>457200</xdr:colOff>
                     <xdr:row>9</xdr:row>
-                    <xdr:rowOff>1133475</xdr:rowOff>
+                    <xdr:rowOff>1136650</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -2037,7 +2761,7 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>0</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>203200</xdr:colOff>
                     <xdr:row>10</xdr:row>
                     <xdr:rowOff>1085850</xdr:rowOff>
                   </from>
@@ -2045,7 +2769,7 @@
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>400050</xdr:colOff>
                     <xdr:row>10</xdr:row>
-                    <xdr:rowOff>1323975</xdr:rowOff>
+                    <xdr:rowOff>1327150</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -2059,9 +2783,9 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>0</xdr:col>
-                    <xdr:colOff>238125</xdr:colOff>
+                    <xdr:colOff>241300</xdr:colOff>
                     <xdr:row>11</xdr:row>
-                    <xdr:rowOff>276225</xdr:rowOff>
+                    <xdr:rowOff>279400</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>0</xdr:col>
@@ -2085,25 +2809,25 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" width="8.625" customWidth="1"/>
-    <col min="2" max="2" width="15.875" customWidth="1"/>
-    <col min="3" max="3" width="19.375" customWidth="1"/>
-    <col min="4" max="4" width="28.375" customWidth="1"/>
-    <col min="5" max="5" width="49.875" customWidth="1"/>
-    <col min="6" max="6" width="40.125" customWidth="1"/>
+    <col min="1" max="1" width="8.58203125" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" customWidth="1"/>
+    <col min="4" max="4" width="28.33203125" customWidth="1"/>
+    <col min="5" max="5" width="49.83203125" customWidth="1"/>
+    <col min="6" max="6" width="40.08203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1">
       <c r="A1" s="2" t="s">
-        <v>47</v>
+        <v>18</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>2</v>
@@ -2118,22 +2842,22 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="5" customFormat="1" ht="93.75">
+    <row r="2" spans="1:6" s="5" customFormat="1" ht="108">
       <c r="A2" s="12" t="b">
         <v>1</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>45</v>
+        <v>16</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="4" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -2154,11 +2878,11 @@
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>228600</xdr:colOff>
                     <xdr:row>1</xdr:row>
-                    <xdr:rowOff>447675</xdr:rowOff>
+                    <xdr:rowOff>450850</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>0</xdr:col>
-                    <xdr:colOff>428625</xdr:colOff>
+                    <xdr:colOff>431800</xdr:colOff>
                     <xdr:row>1</xdr:row>
                     <xdr:rowOff>685800</xdr:rowOff>
                   </to>

</xml_diff>